<commit_message>
added activities to Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicdonaldson/Software Technologies/Assignment/2810ICT-2022-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF8D0076-DE52-7D4B-9911-766ADE50FD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -36,90 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>PERIODS</t>
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -230,40 +153,133 @@
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
-    <t>Project Title</t>
+    <t>Accident Analysis Software</t>
+  </si>
+  <si>
+    <t>1. Conceptualise</t>
+  </si>
+  <si>
+    <t>1.1 Understanding Project Requirements</t>
+  </si>
+  <si>
+    <t>1.2 Outcomes of the Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3 Dataset Decision </t>
+  </si>
+  <si>
+    <t>1.4 Expectations</t>
+  </si>
+  <si>
+    <t>1.5 Github Repository Configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6 Research </t>
+  </si>
+  <si>
+    <t>1.7 Git &amp; Github Training</t>
+  </si>
+  <si>
+    <t>2. Planning</t>
+  </si>
+  <si>
+    <t>2.1 Work Breakdown Structure</t>
+  </si>
+  <si>
+    <t>2.2 Gantt Chart</t>
+  </si>
+  <si>
+    <t>2.3 Project Plan Introduction</t>
+  </si>
+  <si>
+    <t>2.4 Activity Definition &amp; Estimation</t>
+  </si>
+  <si>
+    <t>2.5 System Vision &amp; Requirements</t>
+  </si>
+  <si>
+    <t>2.6 Software and User Interface Design Plan</t>
+  </si>
+  <si>
+    <t>2.7 Part A Submission</t>
+  </si>
+  <si>
+    <t>3. Devlopment</t>
+  </si>
+  <si>
+    <t>3.1 Required Feature 1</t>
+  </si>
+  <si>
+    <t>3.2 Required Feature 2</t>
+  </si>
+  <si>
+    <t>3.3 Required Feature 3</t>
+  </si>
+  <si>
+    <t>3.4 Required Feature 4</t>
+  </si>
+  <si>
+    <t>3.5 Required Feature 5</t>
+  </si>
+  <si>
+    <t>3.6 Software Design</t>
+  </si>
+  <si>
+    <t>3.7 User Interface Design</t>
+  </si>
+  <si>
+    <t>4. Final Prep</t>
+  </si>
+  <si>
+    <t>4.1 Testing Plan</t>
+  </si>
+  <si>
+    <t>4.2 Unit Tests &amp; Coverage Test Results</t>
+  </si>
+  <si>
+    <t>4.3 Update Project Plan</t>
+  </si>
+  <si>
+    <t>4.4 Update System Design Document</t>
+  </si>
+  <si>
+    <t>4.5 Update Gantt Chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.6 Executive Summary </t>
+  </si>
+  <si>
+    <t>4.7 Instruction Booklet/User Manual</t>
+  </si>
+  <si>
+    <t>5. Release</t>
+  </si>
+  <si>
+    <t>5.1 Software Release</t>
+  </si>
+  <si>
+    <t>5.2 Release Analysis</t>
+  </si>
+  <si>
+    <t>5.3 Necessary Updates</t>
+  </si>
+  <si>
+    <t>5.4 Support</t>
+  </si>
+  <si>
+    <t>5.5 Final Check &amp; Consolidation</t>
+  </si>
+  <si>
+    <t>5.6 Part B Submission</t>
+  </si>
+  <si>
+    <t>5.7 Reflection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,42 +634,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -666,35 +688,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="57">
     <dxf>
       <fill>
         <patternFill>
@@ -811,6 +827,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -822,17 +866,545 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
-        </top>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1189,33 +1761,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO39"/>
+  <dimension ref="B1:BO44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="2.83203125" style="1"/>
+    <col min="42" max="42" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1223,23 +1795,23 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="30" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1247,58 +1819,58 @@
       <c r="O2" s="32"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="30" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="V2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="39"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AI2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+    </row>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1323,7 +1895,7 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="26"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1511,9 +2083,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1527,9 +2099,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1539,9 +2111,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1551,9 +2123,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1563,9 +2135,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1575,9 +2147,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1587,9 +2159,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1599,9 +2171,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1611,9 +2183,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1623,9 +2195,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1635,9 +2207,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="7"/>
@@ -1647,9 +2219,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1659,9 +2231,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1671,9 +2243,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1683,9 +2255,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1695,9 +2267,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1707,9 +2279,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1719,9 +2291,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1731,9 +2303,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1743,9 +2315,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1755,9 +2327,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1767,9 +2339,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1779,9 +2351,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1791,9 +2363,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1803,9 +2375,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1815,9 +2387,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1827,9 +2399,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1839,9 +2411,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1851,9 +2423,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1863,9 +2435,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1875,9 +2447,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1887,9 +2459,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1899,9 +2471,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1911,9 +2483,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1923,9 +2495,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1935,70 +2507,260 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="56" priority="49">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="55" priority="51">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="54" priority="52">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="53" priority="53">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="52" priority="54">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="51" priority="55">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="50" priority="59">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="49" priority="60">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="48" priority="56">
       <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40:BO40">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41:BO41">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42:BO42">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:BO43">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44:BO44">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>